<commit_message>
updates HTML for v1, fixes ReSpec metadata
- The version has been changed to v1 in HTML files (RDF is ToDo)
- Each document has a distinct shortName property to enable publishing
  under distinct and unique URIs in CG-reports
- Fixed an error in UCR where a missing concept caused exceptions
- The ReSpec outputs have NOT been exported
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/ucr.xlsx
+++ b/documentation-generator/vocab_csv/ucr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Description of the use-case - a short summary of what/who/how/where/when etc. goes here. This can be as detailed as you want.</t>
   </si>
   <si>
+    <t>dpv:Concept</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
@@ -76,520 +79,520 @@
     <t>Digital resources, e.g., resources stored in Solid pods, might contain multiple types of personal data categories, including sensitive personal data categories. For instance, in the Solid ecossystem, tagging the resources, or their metadata, with the personal data categories they contain will assist in the matching of personal data categories and the access control policies expressed for those particular categories of data.</t>
   </si>
   <si>
-    <t>Personal Data</t>
+    <t>dpv:PersonalData</t>
+  </si>
+  <si>
+    <t>Beatriz Esteves</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>Access control policies</t>
+  </si>
+  <si>
+    <t>DPV can be used to define access control policies over digital resources, independently or together with other languages, e.g., ODRL.</t>
+  </si>
+  <si>
+    <t>dpv:PersonalData,dpv:Purpose,dpv:Entity,dpv:Processing,dpv:LegalBasis,dpv:TechnicalOrganisationalMeasure</t>
+  </si>
+  <si>
+    <t>DPV Concept(s)</t>
+  </si>
+  <si>
+    <t>UseCase(s)</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Dummy Requirement</t>
+  </si>
+  <si>
+    <t>This requirement does not entail anything</t>
+  </si>
+  <si>
+    <t>dpv:Concept,dpv:Relation</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Provide concepts in standardised, consistent, machine-readable form</t>
+  </si>
+  <si>
+    <t>The encapsulation of concepts must be in a form that is machine-readable, consistent, and using a formal specification - ideally a standard. This will ensure the concepts are correctly parsed, interpreted, and used by machines across use-cases, and will assist in the automation of information and information-based tasks.</t>
+  </si>
+  <si>
+    <t>U2,U3</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Provide concepts as a dictionary or thesauri with contextual parts</t>
+  </si>
+  <si>
+    <t>The concepts should be bundled together and provided as a vocabulary or thesauri with distinct parts or sections (or sub-vocabularies) that relate to specific contextual details. For example, providing purposes as a separate taxonomy enables use of only purposes elsewhere.</t>
+  </si>
+  <si>
+    <t>Source path</t>
+  </si>
+  <si>
+    <t>Concepts</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Embed?</t>
+  </si>
+  <si>
+    <t>E0001</t>
+  </si>
+  <si>
+    <t>Dummy Example 1</t>
+  </si>
+  <si>
+    <t>Dummy Example description</t>
+  </si>
+  <si>
+    <t>E0001.ttl</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Harsh</t>
+  </si>
+  <si>
+    <t>E0002</t>
+  </si>
+  <si>
+    <t>Dummy Example 2</t>
+  </si>
+  <si>
+    <t>Dummy Example 2 description</t>
+  </si>
+  <si>
+    <t>E0002.ttl</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>E0003</t>
+  </si>
+  <si>
+    <t>Extending Purpose for Use-Case</t>
+  </si>
+  <si>
+    <t>DPV defines the (broad) concept Marketing in its Purpose hierarchy to represent information about (purposes related to) marketing activities and topics. For a use-case which requires representing purposes (note: plural) related to marketing of new products, the broad Marketing concept is extended as a child or subclass concept for representing the intended purpose as, e.g. MarketingNewProducts.</t>
+  </si>
+  <si>
+    <t>E0003.ttl</t>
+  </si>
+  <si>
+    <t>dpvs:Purpose</t>
+  </si>
+  <si>
+    <t>E0004</t>
+  </si>
+  <si>
+    <t>DPV-OWL: Extending Purpose for Use-Case</t>
+  </si>
+  <si>
+    <t>E0004.ttl</t>
+  </si>
+  <si>
+    <t>dpvo:Purpose</t>
+  </si>
+  <si>
+    <t>E0005</t>
+  </si>
+  <si>
+    <t>Combining concepts to indicate they always occur together</t>
+  </si>
+  <si>
+    <t>Consider the use-case where an activity simultaneously uses the data while collecting it. The first representation (&lt;code&gt;ActivityA&lt;/code&gt;) models them separately - which is not accurate as it is ambiguous in terms of collection and usage taking place independently. By extending the collect and use concepts to create a new concept called &lt;code&gt;CollectAndUse&lt;/code&gt;, it is possible to accurately declare that they both occur as a concurrent operation. Such combinations of concepts are also useful to collectively represent or annotate additional information such as: technologies involved, implementation details, or agents involved</t>
+  </si>
+  <si>
+    <t>E0005.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Concept,dpv:Processing</t>
+  </si>
+  <si>
+    <t>E0006</t>
+  </si>
+  <si>
+    <t>Maintaining Interoperability between Use-Cases</t>
+  </si>
+  <si>
+    <t>For example, two TV companies (&lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt;) extend the concept &lt;code&gt;Optimisation&lt;/code&gt; to reflect their respective purposes. When exchanging information about their use-cases with each other (or with a third party), by following the chain of use-case specific concepts it is possible to deduce that both &lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt; are doing optimisations for consumers. Thus a common language or interface can be developed based on using DPV as a point of interoperability and commonality which can be used by adopters to define the specifics of their use-case. For example, in the above use-case, a common notice generation algorithm could be created and used to inform users of both services the purposes each company is using data for.</t>
+  </si>
+  <si>
+    <t>E0006.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Concept,dpv:Purpose</t>
+  </si>
+  <si>
+    <t>E0007</t>
+  </si>
+  <si>
+    <t>Use of PersonalDataHandling to group how data is being processed</t>
+  </si>
+  <si>
+    <t>For an example of how &lt;code&gt;PersonalDataHandling&lt;/code&gt; brings together the core concepts, consider the example where &lt;code&gt;Acme&lt;/code&gt; is a &lt;code&gt;DataController&lt;/code&gt; that &lt;code&gt;Collect&lt;/code&gt;(s) and &lt;code&gt;Use&lt;/code&gt;(s) &lt;code&gt;Email&lt;/code&gt; for &lt;code&gt;ServiceProvision&lt;/code&gt;.</t>
+  </si>
+  <si>
+    <t>E0007.ttl</t>
+  </si>
+  <si>
+    <t>dpv:PersonalDataHandling</t>
+  </si>
+  <si>
+    <t>E0008</t>
+  </si>
+  <si>
+    <t>Nesting PersonalDataHandling for modular expression of processing operations</t>
+  </si>
+  <si>
+    <t>onsider the example where &lt;em&gt;Acme&lt;/em&gt;, as a &lt;em&gt;DataController&lt;/em&gt;, maintains records of its processing activities using &lt;code&gt;PersonalDataHandling&lt;/code&gt; to represent one of its services. In this, it collects email, uses it for internal analyses based on &lt;em&gt;LegitimateInterests&lt;/em&gt;, and also sends marketing information by using a processor based on the data subject's consent. Using nesting of personal data handling, the information can be expressed at granular level representing service, individual purposes, and so on.</t>
+  </si>
+  <si>
+    <t>E0008.ttl</t>
+  </si>
+  <si>
+    <t>E0009</t>
+  </si>
+  <si>
+    <t>Adding human-readable descriptions</t>
+  </si>
+  <si>
+    <t>In this example, a new purpose is created by extending &lt;code&gt;dpv:FraudPreventionAndDetection&lt;/code&gt; and annotated with human-readable information. The interpretation of this purpose is thus more clear in relation to how it is applied or used within that use-case, and also serves to compare it with other purposes within the same category.</t>
+  </si>
+  <si>
+    <t>E0009.ttl</t>
+  </si>
+  <si>
+    <t>E0010</t>
+  </si>
+  <si>
+    <t>Using NACE codes to restrict Purposes</t>
+  </si>
+  <si>
+    <t>For example, the following purpose concerns implementing access control with the domain specified as scientific research using its corresponding NACE code &lt;code&gt;M72&lt;/code&gt; to indicate sectorial implications for what "access control" and "enforce security" are expected to imply.</t>
+  </si>
+  <si>
+    <t>E0010.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Purpose,dpv:Sector</t>
+  </si>
+  <si>
+    <t>E0011</t>
+  </si>
+  <si>
+    <t>Storage Conditions</t>
+  </si>
+  <si>
+    <t>Acme is a Data Processor that stores data within servers located in Ireland for a period of one year.</t>
+  </si>
+  <si>
+    <t>E0011.ttl</t>
+  </si>
+  <si>
+    <t>dpv:DataProcessor,dpv:Processing,dpv:StorageCondition,dpv:Location,dpv:Duration</t>
+  </si>
+  <si>
+    <t>E0012</t>
+  </si>
+  <si>
+    <t>Data Sources</t>
+  </si>
+  <si>
+    <t>Data sources can be the data subject (direct or indirect), the data controller or processor (itself), or another entity (third party). The below example provides an overview of these with distinctions between source and method of generation.</t>
+  </si>
+  <si>
+    <t>E0012.ttl</t>
+  </si>
+  <si>
+    <t>dpv:DataSource</t>
+  </si>
+  <si>
+    <t>E0013</t>
+  </si>
+  <si>
+    <t>Automated Processing with Human Involvement</t>
+  </si>
+  <si>
+    <t>Consider the use of a spam filter that is based on automated processing operations where humans provide inputs, have oversight of the operation, and results in automated decision making for whether communications should be propogated. A new separate filter is developed that utilises a novel spam detection criteria that also takes into account communications other than emails for the sender and makes automated decisions whether to permit communication to proceed. Such explicit annotation of several high-risk operations assists in performing impact assessments for this technology, as well as understanding the extent and effectiveness of human involvement to mitigate risks and issues.</t>
+  </si>
+  <si>
+    <t>E0013.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ProcessingAutomation,dpv:HumanInput</t>
+  </si>
+  <si>
+    <t>E0014</t>
+  </si>
+  <si>
+    <t>Derivation and inference of personal data</t>
+  </si>
+  <si>
+    <t>This use-case collects browser fingerprint and IP Address to identify the country one is visiting from, and to infer language to be used for personalisation. Note that this example uses [[DPV-PD]] for personal data concepts.</t>
+  </si>
+  <si>
+    <t>E0014.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Purpose,dpv:Processing,dpv:PersonalDataHandling,dpv:Derive,dpv:Infer</t>
+  </si>
+  <si>
+    <t>E0015</t>
+  </si>
+  <si>
+    <t>Indicating personal data is sensitive or special category</t>
+  </si>
+  <si>
+    <t>In this example, the knowledge that blood samples are of type 'special category' can be inferred from the fact that they are a form of &lt;i&gt;Medical Health&lt;/i&gt; which is a 'special category'. However, the example considers best practices that suggest explicitly identifying and denoting that blood samples are also of type 'special category'.</t>
+  </si>
+  <si>
+    <t>E0015.ttl</t>
+  </si>
+  <si>
+    <t>dpv:SpecialCategoryPersonalData,dpv:SensitivePersonalData</t>
+  </si>
+  <si>
+    <t>E0016</t>
+  </si>
+  <si>
+    <t>Protecting data using encryption and access control</t>
+  </si>
+  <si>
+    <t>To indicate data is encrypted using the &lt;a href="https://en.wikipedia.org/wiki/RSA_(cryptosystem)"&gt;Rivest-Shamir-Adleman (RSA) method&lt;/a&gt;, one would extend the &lt;a href="https://www.w3id.org/dpv#Encryption"&gt;&lt;code&gt;Encryption&lt;/code&gt;&lt;/a&gt; concept within DPV to represent &lt;code&gt;RSA&lt;/code&gt;, and then instantiate it with the specific implementation used (e.g. to indicate key size). Access to this data is further restricted by requiring a password or credential.</t>
+  </si>
+  <si>
+    <t>E0016.ttl</t>
+  </si>
+  <si>
+    <t>dpv:TechnicalMeasure,dpv:Encryption,dpv:AccessControlMethod</t>
+  </si>
+  <si>
+    <t>E0017</t>
+  </si>
+  <si>
+    <t>Indicating staff training for use of Credentials</t>
+  </si>
+  <si>
+    <t>To indicate staff are trained in the use of credentials, and that a policy exists regarding this, the use of &lt;code&gt;OrganisationalMeasure&lt;/code&gt; concepts can be combined in several ways. Note that the interpretations for how staff training is associated with credentials, or contains training regarding credentials is arbitrary in notation. It is intended to demonstrate how different perspectives can be represented so as to be suitable to the organisation's documentation practices.</t>
+  </si>
+  <si>
+    <t>E0017.ttl</t>
+  </si>
+  <si>
+    <t>dpv:OrganisationalMeasure,dpv:StaffTraining,dpv:Policy</t>
+  </si>
+  <si>
+    <t>E0018</t>
+  </si>
+  <si>
+    <t>Notice used in an activity</t>
+  </si>
+  <si>
+    <t>This example first specifies a privacy notice as a document is being used in the context of a service as represented using a personal data handling instance. Then it provides an alternative representation where the contents of a notice are described using DPV.</t>
+  </si>
+  <si>
+    <t>E0018.ttl</t>
+  </si>
+  <si>
+    <t>dpv:PersonalDataHandling,dpv:PrivacyNotice,dpv:ServiceProvision,dpv:Collect</t>
+  </si>
+  <si>
+    <t>E0019</t>
+  </si>
+  <si>
+    <t>Consent record</t>
+  </si>
+  <si>
+    <t>This example shows a consent record containing the topic of consent (i.e. which processing activities it was about), its current status, and when it was given by the data subject. The structure of a record is highly dependant on the requirements of the use-case, and can vary across implementations. In this case, it is based on a draft of the ISO/IEC AWI TS 27560 Privacy technologies - Consent record information structure.</t>
+  </si>
+  <si>
+    <t>E0019.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ConsentRecord,dpv:PersonalDataHandling,dpv:Consent,dpv:DataController,dpv:Jurisdiction,dpv:Recipient,dpv:ConsentStatus,dpv:ConsentType,dpv:Duration</t>
+  </si>
+  <si>
+    <t>E0020</t>
+  </si>
+  <si>
+    <t>Controller-Processor agreement</t>
+  </si>
+  <si>
+    <t>Acme is the Data Controller, that contracts BetaInc as a Data Processor to analyse raw call logs and provide statistical patterns.</t>
+  </si>
+  <si>
+    <t>E0020.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Controller,dpv:Processor,dpv:ControllerProcessorAgreement,dpv:PersonalDataHandling,dpv:Transfer,dpv:DataSource</t>
+  </si>
+  <si>
+    <t>E0021</t>
+  </si>
+  <si>
+    <t>Data transfer safeguards</t>
+  </si>
+  <si>
+    <t>This example represents a contractual agreement between a controller and a processor indicating the use of encryption and EU commission approved Standard Contractual Clauses as specific measures to safeguard data transfers between them.</t>
+  </si>
+  <si>
+    <t>E0021.ttl</t>
+  </si>
+  <si>
+    <t>dpv:ControllerProcessorAgreement,dpv:DataTransferSafeguard,dpv-gdpr:SCCsByCommission</t>
+  </si>
+  <si>
+    <t>E0022</t>
+  </si>
+  <si>
+    <t>Denoting Legal Basis</t>
+  </si>
+  <si>
+    <t>The &lt;code&gt;LegalBasis&lt;/code&gt; can be associated with any concept using the relation &lt;code&gt;hasLegalBasis&lt;/code&gt;. Such associations are of three types: (1) where the legal basis refers to an instance, such as the consent or contract associated with a particular data subject; (2) where the legal basis refers to the category that will be used to justify processing, such as the concept &lt;i&gt;consent&lt;/i&gt; to denote consent will be the basis for indicated processing; and lastly (3) where the legal basis is the denoted with context, such as &lt;i&gt;consent of service consumers&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>E0022.ttl</t>
+  </si>
+  <si>
+    <t>dpv:LegalBasis,dpv:PersonalDataHandling,dpv:Consent</t>
+  </si>
+  <si>
+    <t>E0023</t>
+  </si>
+  <si>
+    <t>Consent as legal basis</t>
+  </si>
+  <si>
+    <t>Here, a personal data handling instance represents some context (e.g. a service, or a product, or some opreation), and the example specifies that the legal basis for these is the use of consent.</t>
+  </si>
+  <si>
+    <t>E0023.ttl</t>
+  </si>
+  <si>
+    <t>dpv:LegalBasis,dpv:Consent</t>
+  </si>
+  <si>
+    <t>E0024</t>
+  </si>
+  <si>
+    <t>Details of Consent</t>
+  </si>
+  <si>
+    <t>In this example, an individual's consent is recorded with abstraction in the form of linking to a common personal data handling instance from the previous example. This 'common' personal data handling represents processing taking place for all data subjects, whereas the consent instance refers only to the individual with a link to this common information. This is to present an alternative method for storing information as compared to extensive consent records.</t>
+  </si>
+  <si>
+    <t>E0024.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Consent,dpv:ConsentStatus,dpv:ConsentType</t>
+  </si>
+  <si>
+    <t>E0025</t>
+  </si>
+  <si>
+    <t>Consent Notice</t>
+  </si>
+  <si>
+    <t>Representing notice, provision, expiry, and withdrawal information for consent</t>
+  </si>
+  <si>
+    <t>E0025.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Consent,dpv:ConsentStatus,dpv:ConsentType,dpv:Notice,dpv:PrivacyNotice</t>
+  </si>
+  <si>
+    <t>E0026</t>
+  </si>
+  <si>
+    <t>Using consent types</t>
+  </si>
+  <si>
+    <t>Expressing consent type is required as legal basis and as instances</t>
+  </si>
+  <si>
+    <t>E0026.ttl</t>
+  </si>
+  <si>
+    <t>E0027</t>
+  </si>
+  <si>
+    <t>Describing Entities</t>
+  </si>
+  <si>
+    <t>Indicating Entity Information, including DPO and Representatives</t>
+  </si>
+  <si>
+    <t>E0027.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Entity</t>
+  </si>
+  <si>
+    <t>E0028</t>
+  </si>
+  <si>
+    <t>Contextual Necessity</t>
+  </si>
+  <si>
+    <t>In this example, a &lt;code&gt;PersonalDataHandling&lt;/code&gt; instance is comprised of two nested &lt;code&gt;PersonalDataHandling&lt;/code&gt; instances for each of the optional and required parts. The personal data category 'Account Identifier' is indicated as being required for 'Communication for Customer Care', while the use of 'Email' is optional for the same purpose.</t>
+  </si>
+  <si>
+    <t>E0028.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Context,dpv:Necessity,dpv:PersonalDataHandling</t>
+  </si>
+  <si>
+    <t>E0029</t>
+  </si>
+  <si>
+    <t>Risk and Consequence</t>
+  </si>
+  <si>
+    <t>In this example, we consider &lt;i&gt;Risk&lt;/i&gt; can be associated with any concept given its broad existence and applicability, and that its mitigation is a technical and organisational measure. Using this, the implemented or adopted technical and organisational measures within an use-case are annotated with the risks they address or mitigate, along with specific impacts that may occur if the risk were to occur. For example, the storage of personal data within a database has an implementation of access control that mitigates the consequence of unauthorised access and its impact to cause harm.</t>
+  </si>
+  <si>
+    <t>E0029.ttl</t>
+  </si>
+  <si>
+    <t>dpv:Riskl,dpv:Consequence,dpv:Impact,dpv:Harm,dpv:RiskMitigationMeasure</t>
+  </si>
+  <si>
+    <t>EXAMPLE</t>
+  </si>
+  <si>
+    <t>Provide example code / description</t>
+  </si>
+  <si>
+    <t>Users' privacy preferences</t>
+  </si>
+  <si>
+    <t>Indicating information regarding users' privacy preferences</t>
+  </si>
+  <si>
+    <t>dpv:PrivacyPreference</t>
   </si>
   <si>
     <t>beatriz</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>Access control policies</t>
-  </si>
-  <si>
-    <t>DPV can be used to define access control policies over digital resources, independently or together with other languages, e.g., ODRL.</t>
-  </si>
-  <si>
-    <t>Personal Data, Purposes, Entities, Processing, Legal Basis, Technical and Organisational Measures</t>
-  </si>
-  <si>
-    <t>DPV Concept(s)</t>
-  </si>
-  <si>
-    <t>UseCase(s)</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>Dummy Requirement</t>
-  </si>
-  <si>
-    <t>This requirement does not entail anything</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Provide concepts in standardised, consistent, machine-readable form</t>
-  </si>
-  <si>
-    <t>The encapsulation of concepts must be in a form that is machine-readable, consistent, and using a formal specification - ideally a standard. This will ensure the concepts are correctly parsed, interpreted, and used by machines across use-cases, and will assist in the automation of information and information-based tasks.</t>
-  </si>
-  <si>
-    <t>dpv:Concept,dpv:Relation</t>
-  </si>
-  <si>
-    <t>U2,U3</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>Provide concepts as a dictionary or thesauri with contextual parts</t>
-  </si>
-  <si>
-    <t>The concepts should be bundled together and provided as a vocabulary or thesauri with distinct parts or sections (or sub-vocabularies) that relate to specific contextual details. For example, providing purposes as a separate taxonomy enables use of only purposes elsewhere.</t>
-  </si>
-  <si>
-    <t>Source path</t>
-  </si>
-  <si>
-    <t>Concepts</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Embed?</t>
-  </si>
-  <si>
-    <t>E0001</t>
-  </si>
-  <si>
-    <t>Dummy Example 1</t>
-  </si>
-  <si>
-    <t>Dummy Example description</t>
-  </si>
-  <si>
-    <t>E0001.ttl</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Harsh</t>
-  </si>
-  <si>
-    <t>E0002</t>
-  </si>
-  <si>
-    <t>Dummy Example 2</t>
-  </si>
-  <si>
-    <t>Dummy Example 2 description</t>
-  </si>
-  <si>
-    <t>E0002.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Concept</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>E0003</t>
-  </si>
-  <si>
-    <t>Extending Purpose for Use-Case</t>
-  </si>
-  <si>
-    <t>DPV defines the (broad) concept Marketing in its Purpose hierarchy to represent information about (purposes related to) marketing activities and topics. For a use-case which requires representing purposes (note: plural) related to marketing of new products, the broad Marketing concept is extended as a child or subclass concept for representing the intended purpose as, e.g. MarketingNewProducts.</t>
-  </si>
-  <si>
-    <t>E0003.ttl</t>
-  </si>
-  <si>
-    <t>dpvs:Purpose</t>
-  </si>
-  <si>
-    <t>E0004</t>
-  </si>
-  <si>
-    <t>DPV-OWL: Extending Purpose for Use-Case</t>
-  </si>
-  <si>
-    <t>E0004.ttl</t>
-  </si>
-  <si>
-    <t>dpvo:Purpose</t>
-  </si>
-  <si>
-    <t>E0005</t>
-  </si>
-  <si>
-    <t>Combining concepts to indicate they always occur together</t>
-  </si>
-  <si>
-    <t>Consider the use-case where an activity simultaneously uses the data while collecting it. The first representation (&lt;code&gt;ActivityA&lt;/code&gt;) models them separately - which is not accurate as it is ambiguous in terms of collection and usage taking place independently. By extending the collect and use concepts to create a new concept called &lt;code&gt;CollectAndUse&lt;/code&gt;, it is possible to accurately declare that they both occur as a concurrent operation. Such combinations of concepts are also useful to collectively represent or annotate additional information such as: technologies involved, implementation details, or agents involved</t>
-  </si>
-  <si>
-    <t>E0005.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Concept,dpv:Processing</t>
-  </si>
-  <si>
-    <t>E0006</t>
-  </si>
-  <si>
-    <t>Maintaining Interoperability between Use-Cases</t>
-  </si>
-  <si>
-    <t>For example, two TV companies (&lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt;) extend the concept &lt;code&gt;Optimisation&lt;/code&gt; to reflect their respective purposes. When exchanging information about their use-cases with each other (or with a third party), by following the chain of use-case specific concepts it is possible to deduce that both &lt;code&gt;AliceCo&lt;/code&gt; and &lt;code&gt;BobCo&lt;/code&gt; are doing optimisations for consumers. Thus a common language or interface can be developed based on using DPV as a point of interoperability and commonality which can be used by adopters to define the specifics of their use-case. For example, in the above use-case, a common notice generation algorithm could be created and used to inform users of both services the purposes each company is using data for.</t>
-  </si>
-  <si>
-    <t>E0006.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Concept,dpv:Purpose</t>
-  </si>
-  <si>
-    <t>E0007</t>
-  </si>
-  <si>
-    <t>Use of PersonalDataHandling to group how data is being processed</t>
-  </si>
-  <si>
-    <t>For an example of how &lt;code&gt;PersonalDataHandling&lt;/code&gt; brings together the core concepts, consider the example where &lt;code&gt;Acme&lt;/code&gt; is a &lt;code&gt;DataController&lt;/code&gt; that &lt;code&gt;Collect&lt;/code&gt;(s) and &lt;code&gt;Use&lt;/code&gt;(s) &lt;code&gt;Email&lt;/code&gt; for &lt;code&gt;ServiceProvision&lt;/code&gt;.</t>
-  </si>
-  <si>
-    <t>E0007.ttl</t>
-  </si>
-  <si>
-    <t>dpv:PersonalDataHandling</t>
-  </si>
-  <si>
-    <t>E0008</t>
-  </si>
-  <si>
-    <t>Nesting PersonalDataHandling for modular expression of processing operations</t>
-  </si>
-  <si>
-    <t>onsider the example where &lt;em&gt;Acme&lt;/em&gt;, as a &lt;em&gt;DataController&lt;/em&gt;, maintains records of its processing activities using &lt;code&gt;PersonalDataHandling&lt;/code&gt; to represent one of its services. In this, it collects email, uses it for internal analyses based on &lt;em&gt;LegitimateInterests&lt;/em&gt;, and also sends marketing information by using a processor based on the data subject's consent. Using nesting of personal data handling, the information can be expressed at granular level representing service, individual purposes, and so on.</t>
-  </si>
-  <si>
-    <t>E0008.ttl</t>
-  </si>
-  <si>
-    <t>E0009</t>
-  </si>
-  <si>
-    <t>Adding human-readable descriptions</t>
-  </si>
-  <si>
-    <t>In this example, a new purpose is created by extending &lt;code&gt;dpv:FraudPreventionAndDetection&lt;/code&gt; and annotated with human-readable information. The interpretation of this purpose is thus more clear in relation to how it is applied or used within that use-case, and also serves to compare it with other purposes within the same category.</t>
-  </si>
-  <si>
-    <t>E0009.ttl</t>
-  </si>
-  <si>
-    <t>E0010</t>
-  </si>
-  <si>
-    <t>Using NACE codes to restrict Purposes</t>
-  </si>
-  <si>
-    <t>For example, the following purpose concerns implementing access control with the domain specified as scientific research using its corresponding NACE code &lt;code&gt;M72&lt;/code&gt; to indicate sectorial implications for what "access control" and "enforce security" are expected to imply.</t>
-  </si>
-  <si>
-    <t>E0010.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Purpose,dpv:Sector</t>
-  </si>
-  <si>
-    <t>E0011</t>
-  </si>
-  <si>
-    <t>Storage Conditions</t>
-  </si>
-  <si>
-    <t>Acme is a Data Processor that stores data within servers located in Ireland for a period of one year.</t>
-  </si>
-  <si>
-    <t>E0011.ttl</t>
-  </si>
-  <si>
-    <t>dpv:DataProcessor,dpv:Processing,dpv:StorageCondition,dpv:Location,dpv:Duration</t>
-  </si>
-  <si>
-    <t>E0012</t>
-  </si>
-  <si>
-    <t>Data Sources</t>
-  </si>
-  <si>
-    <t>Data sources can be the data subject (direct or indirect), the data controller or processor (itself), or another entity (third party). The below example provides an overview of these with distinctions between source and method of generation.</t>
-  </si>
-  <si>
-    <t>E0012.ttl</t>
-  </si>
-  <si>
-    <t>dpv:DataSource</t>
-  </si>
-  <si>
-    <t>E0013</t>
-  </si>
-  <si>
-    <t>Automated Processing with Human Involvement</t>
-  </si>
-  <si>
-    <t>Consider the use of a spam filter that is based on automated processing operations where humans provide inputs, have oversight of the operation, and results in automated decision making for whether communications should be propogated. A new separate filter is developed that utilises a novel spam detection criteria that also takes into account communications other than emails for the sender and makes automated decisions whether to permit communication to proceed. Such explicit annotation of several high-risk operations assists in performing impact assessments for this technology, as well as understanding the extent and effectiveness of human involvement to mitigate risks and issues.</t>
-  </si>
-  <si>
-    <t>E0013.ttl</t>
-  </si>
-  <si>
-    <t>dpv:ProcessingAutomation,dpv:HumanInput</t>
-  </si>
-  <si>
-    <t>E0014</t>
-  </si>
-  <si>
-    <t>Derivation and inference of personal data</t>
-  </si>
-  <si>
-    <t>This use-case collects browser fingerprint and IP Address to identify the country one is visiting from, and to infer language to be used for personalisation. Note that this example uses [[DPV-PD]] for personal data concepts.</t>
-  </si>
-  <si>
-    <t>E0014.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Purpose,dpv:Processing,dpv:PersonalDataHandling,dpv:Derive,dpv:Infer</t>
-  </si>
-  <si>
-    <t>E0015</t>
-  </si>
-  <si>
-    <t>Indicating personal data is sensitive or special category</t>
-  </si>
-  <si>
-    <t>In this example, the knowledge that blood samples are of type 'special category' can be inferred from the fact that they are a form of &lt;i&gt;Medical Health&lt;/i&gt; which is a 'special category'. However, the example considers best practices that suggest explicitly identifying and denoting that blood samples are also of type 'special category'.</t>
-  </si>
-  <si>
-    <t>E0015.ttl</t>
-  </si>
-  <si>
-    <t>dpv:SpecialCategoryPersonalData,dpv:SensitivePersonalData</t>
-  </si>
-  <si>
-    <t>E0016</t>
-  </si>
-  <si>
-    <t>Protecting data using encryption and access control</t>
-  </si>
-  <si>
-    <t>To indicate data is encrypted using the &lt;a href="https://en.wikipedia.org/wiki/RSA_(cryptosystem)"&gt;Rivest-Shamir-Adleman (RSA) method&lt;/a&gt;, one would extend the &lt;a href="https://www.w3id.org/dpv#Encryption"&gt;&lt;code&gt;Encryption&lt;/code&gt;&lt;/a&gt; concept within DPV to represent &lt;code&gt;RSA&lt;/code&gt;, and then instantiate it with the specific implementation used (e.g. to indicate key size). Access to this data is further restricted by requiring a password or credential.</t>
-  </si>
-  <si>
-    <t>E0016.ttl</t>
-  </si>
-  <si>
-    <t>dpv:TechnicalMeasure,dpv:Encryption,dpv:AccessControlMethod</t>
-  </si>
-  <si>
-    <t>E0017</t>
-  </si>
-  <si>
-    <t>Indicating staff training for use of Credentials</t>
-  </si>
-  <si>
-    <t>To indicate staff are trained in the use of credentials, and that a policy exists regarding this, the use of &lt;code&gt;OrganisationalMeasure&lt;/code&gt; concepts can be combined in several ways. Note that the interpretations for how staff training is associated with credentials, or contains training regarding credentials is arbitrary in notation. It is intended to demonstrate how different perspectives can be represented so as to be suitable to the organisation's documentation practices.</t>
-  </si>
-  <si>
-    <t>E0017.ttl</t>
-  </si>
-  <si>
-    <t>dpv:OrganisationalMeasure,dpv:StaffTraining,dpv:Policy</t>
-  </si>
-  <si>
-    <t>E0018</t>
-  </si>
-  <si>
-    <t>Notice used in an activity</t>
-  </si>
-  <si>
-    <t>This example first specifies a privacy notice as a document is being used in the context of a service as represented using a personal data handling instance. Then it provides an alternative representation where the contents of a notice are described using DPV.</t>
-  </si>
-  <si>
-    <t>E0018.ttl</t>
-  </si>
-  <si>
-    <t>dpv:PersonalDataHandling,dpv:PrivacyNotice,dpv:ServiceProvision,dpv:Collect</t>
-  </si>
-  <si>
-    <t>E0019</t>
-  </si>
-  <si>
-    <t>Consent record</t>
-  </si>
-  <si>
-    <t>This example shows a consent record containing the topic of consent (i.e. which processing activities it was about), its current status, and when it was given by the data subject. The structure of a record is highly dependant on the requirements of the use-case, and can vary across implementations. In this case, it is based on a draft of the ISO/IEC AWI TS 27560 Privacy technologies - Consent record information structure.</t>
-  </si>
-  <si>
-    <t>E0019.ttl</t>
-  </si>
-  <si>
-    <t>dpv:ConsentRecord,dpv:PersonalDataHandling,dpv:Consent,dpv:DataController,dpv:Jurisdiction,dpv:Recipient,dpv:ConsentStatus,dpv:ConsentType,dpv:Duration</t>
-  </si>
-  <si>
-    <t>E0020</t>
-  </si>
-  <si>
-    <t>Controller-Processor agreement</t>
-  </si>
-  <si>
-    <t>Acme is the Data Controller, that contracts BetaInc as a Data Processor to analyse raw call logs and provide statistical patterns.</t>
-  </si>
-  <si>
-    <t>E0020.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Controller,dpv:Processor,dpv:ControllerProcessorAgreement,dpv:PersonalDataHandling,dpv:Transfer,dpv:DataSource</t>
-  </si>
-  <si>
-    <t>E0021</t>
-  </si>
-  <si>
-    <t>Data transfer safeguards</t>
-  </si>
-  <si>
-    <t>This example represents a contractual agreement between a controller and a processor indicating the use of encryption and EU commission approved Standard Contractual Clauses as specific measures to safeguard data transfers between them.</t>
-  </si>
-  <si>
-    <t>E0021.ttl</t>
-  </si>
-  <si>
-    <t>dpv:ControllerProcessorAgreement,dpv:DataTransferSafeguard,dpv-gdpr:SCCsByCommission</t>
-  </si>
-  <si>
-    <t>E0022</t>
-  </si>
-  <si>
-    <t>Denoting Legal Basis</t>
-  </si>
-  <si>
-    <t>The &lt;code&gt;LegalBasis&lt;/code&gt; can be associated with any concept using the relation &lt;code&gt;hasLegalBasis&lt;/code&gt;. Such associations are of three types: (1) where the legal basis refers to an instance, such as the consent or contract associated with a particular data subject; (2) where the legal basis refers to the category that will be used to justify processing, such as the concept &lt;i&gt;consent&lt;/i&gt; to denote consent will be the basis for indicated processing; and lastly (3) where the legal basis is the denoted with context, such as &lt;i&gt;consent of service consumers&lt;/i&gt;.</t>
-  </si>
-  <si>
-    <t>E0022.ttl</t>
-  </si>
-  <si>
-    <t>dpv:LegalBasis,dpv:PersonalDataHandling,dpv:Consent</t>
-  </si>
-  <si>
-    <t>E0023</t>
-  </si>
-  <si>
-    <t>Consent as legal basis</t>
-  </si>
-  <si>
-    <t>Here, a personal data handling instance represents some context (e.g. a service, or a product, or some opreation), and the example specifies that the legal basis for these is the use of consent.</t>
-  </si>
-  <si>
-    <t>E0023.ttl</t>
-  </si>
-  <si>
-    <t>dpv:LegalBasis,dpv:Consent</t>
-  </si>
-  <si>
-    <t>E0024</t>
-  </si>
-  <si>
-    <t>Details of Consent</t>
-  </si>
-  <si>
-    <t>In this example, an individual's consent is recorded with abstraction in the form of linking to a common personal data handling instance from the previous example. This 'common' personal data handling represents processing taking place for all data subjects, whereas the consent instance refers only to the individual with a link to this common information. This is to present an alternative method for storing information as compared to extensive consent records.</t>
-  </si>
-  <si>
-    <t>E0024.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Consent,dpv:ConsentStatus,dpv:ConsentType</t>
-  </si>
-  <si>
-    <t>E0025</t>
-  </si>
-  <si>
-    <t>Consent Notice</t>
-  </si>
-  <si>
-    <t>Representing notice, provision, expiry, and withdrawal information for consent</t>
-  </si>
-  <si>
-    <t>E0025.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Consent,dpv:ConsentStatus,dpv:ConsentType,dpv:Notice,dpv:PrivacyNotice</t>
-  </si>
-  <si>
-    <t>E0026</t>
-  </si>
-  <si>
-    <t>Using consent types</t>
-  </si>
-  <si>
-    <t>Expressing consent type is required as legal basis and as instances</t>
-  </si>
-  <si>
-    <t>E0026.ttl</t>
-  </si>
-  <si>
-    <t>E0027</t>
-  </si>
-  <si>
-    <t>Describing Entities</t>
-  </si>
-  <si>
-    <t>Indicating Entity Information, including DPO and Representatives</t>
-  </si>
-  <si>
-    <t>E0027.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Entity</t>
-  </si>
-  <si>
-    <t>E0028</t>
-  </si>
-  <si>
-    <t>Contextual Necessity</t>
-  </si>
-  <si>
-    <t>In this example, a &lt;code&gt;PersonalDataHandling&lt;/code&gt; instance is comprised of two nested &lt;code&gt;PersonalDataHandling&lt;/code&gt; instances for each of the optional and required parts. The personal data category 'Account Identifier' is indicated as being required for 'Communication for Customer Care', while the use of 'Email' is optional for the same purpose.</t>
-  </si>
-  <si>
-    <t>E0028.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Context,dpv:Necessity,dpv:PersonalDataHandling</t>
-  </si>
-  <si>
-    <t>E0029</t>
-  </si>
-  <si>
-    <t>Risk and Consequence</t>
-  </si>
-  <si>
-    <t>In this example, we consider &lt;i&gt;Risk&lt;/i&gt; can be associated with any concept given its broad existence and applicability, and that its mitigation is a technical and organisational measure. Using this, the implemented or adopted technical and organisational measures within an use-case are annotated with the risks they address or mitigate, along with specific impacts that may occur if the risk were to occur. For example, the storage of personal data within a database has an implementation of access control that mitigates the consequence of unauthorised access and its impact to cause harm.</t>
-  </si>
-  <si>
-    <t>E0029.ttl</t>
-  </si>
-  <si>
-    <t>dpv:Riskl,dpv:Consequence,dpv:Impact,dpv:Harm,dpv:RiskMitigationMeasure</t>
-  </si>
-  <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>Provide example code / description</t>
-  </si>
-  <si>
-    <t>Users' privacy preferences</t>
-  </si>
-  <si>
-    <t>Indicating information regarding users' privacy preferences</t>
-  </si>
-  <si>
-    <t>dpv:PrivacyPreference</t>
   </si>
 </sst>
 </file>
@@ -967,61 +970,70 @@
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1056,10 +1068,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -1088,13 +1100,16 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -1102,33 +1117,36 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1164,16 +1182,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1201,31 +1219,31 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H2" s="6">
         <v>44846.0</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -1247,22 +1265,22 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>55</v>
@@ -1271,7 +1289,7 @@
         <v>44846.0</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1308,16 +1326,16 @@
         <v>60</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" s="8">
         <v>44847.0</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -1337,16 +1355,16 @@
         <v>64</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H5" s="10">
         <v>44847.0</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1366,16 +1384,16 @@
         <v>69</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H6" s="8">
         <v>44847.0</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -1395,16 +1413,16 @@
         <v>74</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H7" s="10">
         <v>44847.0</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
@@ -1424,16 +1442,16 @@
         <v>79</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H8" s="8">
         <v>44847.0</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9">
@@ -1453,16 +1471,16 @@
         <v>79</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" s="10">
         <v>44847.0</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
@@ -1482,16 +1500,16 @@
         <v>74</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" s="8">
         <v>44847.0</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11">
@@ -1511,16 +1529,16 @@
         <v>92</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H11" s="10">
         <v>44847.0</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -1540,16 +1558,16 @@
         <v>97</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H12" s="8">
         <v>44847.0</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -1569,16 +1587,16 @@
         <v>102</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" s="10">
         <v>44847.0</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
@@ -1598,16 +1616,16 @@
         <v>107</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" s="8">
         <v>44847.0</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
@@ -1627,16 +1645,16 @@
         <v>112</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H15" s="10">
         <v>44847.0</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16">
@@ -1656,16 +1674,16 @@
         <v>117</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H16" s="8">
         <v>44847.0</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
@@ -1685,16 +1703,16 @@
         <v>122</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="10">
         <v>44847.0</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
@@ -1714,16 +1732,16 @@
         <v>127</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H18" s="8">
         <v>44847.0</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
@@ -1743,16 +1761,16 @@
         <v>132</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H19" s="10">
         <v>44847.0</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
@@ -1772,16 +1790,16 @@
         <v>137</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H20" s="8">
         <v>44847.0</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21">
@@ -1801,16 +1819,16 @@
         <v>142</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H21" s="10">
         <v>44847.0</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
@@ -1830,16 +1848,16 @@
         <v>147</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H22" s="8">
         <v>44847.0</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
@@ -1859,16 +1877,16 @@
         <v>152</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H23" s="10">
         <v>44847.0</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24">
@@ -1888,16 +1906,16 @@
         <v>157</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" s="8">
         <v>44847.0</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25">
@@ -1917,16 +1935,16 @@
         <v>162</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H25" s="10">
         <v>44847.0</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26">
@@ -1946,16 +1964,16 @@
         <v>167</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H26" s="8">
         <v>44847.0</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27">
@@ -1975,16 +1993,16 @@
         <v>162</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H27" s="10">
         <v>44847.0</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -2004,16 +2022,16 @@
         <v>176</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H28" s="8">
         <v>44847.0</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29">
@@ -2033,16 +2051,16 @@
         <v>181</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H29" s="10">
         <v>44847.0</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30">
@@ -2062,16 +2080,16 @@
         <v>186</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H30" s="8">
         <v>44847.0</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2106,7 +2124,7 @@
         <v>191</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>21</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>